<commit_message>
added domestic and bay size constraints
</commit_message>
<xml_diff>
--- a/Operations.xlsx
+++ b/Operations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Documents\lr\MSc\operations\github optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0874F789-BC98-49AB-AACC-B391AC401DE1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3417A3F1-9642-4C1C-A08A-E14824D0B2E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bays" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Connections" sheetId="3" r:id="rId3"/>
     <sheet name="walking time" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -745,7 +745,9 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1520,7 +1522,9 @@
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2590,7 +2594,7 @@
   </sheetPr>
   <dimension ref="A1:BK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT13" workbookViewId="0">
+    <sheetView topLeftCell="AT16" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
@@ -14637,7 +14641,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:46" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
@@ -14774,7 +14778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:46" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
         <v>52</v>

</xml_diff>